<commit_message>
starting to populate right info into new database, apply_check
</commit_message>
<xml_diff>
--- a/app/Vendor/db/schema/routes.xlsx
+++ b/app/Vendor/db/schema/routes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="615" windowWidth="21435" windowHeight="7500"/>
+    <workbookView xWindow="870" yWindow="270" windowWidth="12825" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="routes" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="55">
   <si>
     <t>Others</t>
   </si>
@@ -91,9 +91,6 @@
     <t>承認者部門CD</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
     <t>役職区分</t>
   </si>
   <si>
@@ -173,6 +170,15 @@
   </si>
   <si>
     <t>PRI</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>int(5)</t>
+  </si>
+  <si>
+    <t>approverTitle</t>
   </si>
 </sst>
 </file>
@@ -1001,32 +1007,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>50</v>
-      </c>
-      <c r="F1" t="s">
-        <v>51</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1043,7 +1054,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -1080,42 +1091,27 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
@@ -1126,10 +1122,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -1149,13 +1145,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -1172,10 +1168,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -1184,7 +1180,7 @@
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="s">
         <v>4</v>
@@ -1195,13 +1191,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -1218,10 +1214,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -1241,10 +1237,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
@@ -1253,7 +1249,7 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" t="s">
         <v>4</v>
@@ -1264,13 +1260,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
@@ -1287,10 +1283,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -1310,10 +1306,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -1322,7 +1318,7 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="s">
         <v>4</v>
@@ -1333,19 +1329,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F15" t="s">
         <v>4</v>
@@ -1356,10 +1352,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -1379,13 +1375,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
         <v>4</v>
@@ -1402,13 +1398,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
@@ -1425,24 +1421,47 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
         <v>44</v>
       </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>